<commit_message>
Achter les 1 + Strings Domain en MVC
</commit_message>
<xml_diff>
--- a/strings.xlsx
+++ b/strings.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="17571"/>
-  <workbookPr defaultThemeVersion="166925"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="16925"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Jorden Laureyssens\Documents\KdG\16-17\Programmeren\C#-.NET\2-Onderzoekstopics\A - Globalization\Eg_SupportCenter-WebAPI\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Seppe\Source\Repos\Eg_SupportCenter-WebAPI\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="129" uniqueCount="121">
   <si>
     <t>Nederlands</t>
   </si>
@@ -36,6 +36,360 @@
   </si>
   <si>
     <t>StringName</t>
+  </si>
+  <si>
+    <t>"Er zijn maximaal 100 tekens toegestaan"</t>
+  </si>
+  <si>
+    <t>D_t_ErrorMessage</t>
+  </si>
+  <si>
+    <t>"There is a maximum of 100 characters allowed"</t>
+  </si>
+  <si>
+    <t>D_tr_ValidationResult</t>
+  </si>
+  <si>
+    <t>"Can't be before the date the ticket is created!"</t>
+  </si>
+  <si>
+    <t>D_tr_DateString</t>
+  </si>
+  <si>
+    <t>"Date"</t>
+  </si>
+  <si>
+    <t>"Datum"</t>
+  </si>
+  <si>
+    <t>"Kan niet voor de datum dat het ticket is gecreërd!"</t>
+  </si>
+  <si>
+    <t>MVC_trc_BadRequest</t>
+  </si>
+  <si>
+    <t>"Er is iets misgelopen bij het registreren van het antwoord!"</t>
+  </si>
+  <si>
+    <t>"There went something wrong with the registration of the answer!"</t>
+  </si>
+  <si>
+    <t>MVC_hc_AboutMessage</t>
+  </si>
+  <si>
+    <t>"Your application description page."</t>
+  </si>
+  <si>
+    <t>MVC_hc_ContactMessage</t>
+  </si>
+  <si>
+    <t>"Your contact page."</t>
+  </si>
+  <si>
+    <t>"Je contactpagina."</t>
+  </si>
+  <si>
+    <t>"Je applicatie descriptiepagina."</t>
+  </si>
+  <si>
+    <t>"About"</t>
+  </si>
+  <si>
+    <t>"Over"</t>
+  </si>
+  <si>
+    <t>"Contact"</t>
+  </si>
+  <si>
+    <t>"Use this area to provide additional information."</t>
+  </si>
+  <si>
+    <t>"Gebruik dit gebied om extra informatie te verschaffen."</t>
+  </si>
+  <si>
+    <t>"Phone"</t>
+  </si>
+  <si>
+    <t>"Telefoon"</t>
+  </si>
+  <si>
+    <t>"P:"</t>
+  </si>
+  <si>
+    <t>"T:"</t>
+  </si>
+  <si>
+    <t>"Support:"</t>
+  </si>
+  <si>
+    <t>"Ondersteuning:"</t>
+  </si>
+  <si>
+    <t>"Marketing:"</t>
+  </si>
+  <si>
+    <t>"Verkoop:"</t>
+  </si>
+  <si>
+    <t>"Welkom"</t>
+  </si>
+  <si>
+    <t>"Welcome"</t>
+  </si>
+  <si>
+    <t>"SupportCenter"</t>
+  </si>
+  <si>
+    <t>"Helpcentrum"</t>
+  </si>
+  <si>
+    <t>"Welcome on the online helpdesk system."</t>
+  </si>
+  <si>
+    <t>"Welkom op het online helpdesk systeem."</t>
+  </si>
+  <si>
+    <t>"New ticket"</t>
+  </si>
+  <si>
+    <t>"Nieuw ticket"</t>
+  </si>
+  <si>
+    <t>"Create a new ticket in the system."</t>
+  </si>
+  <si>
+    <t>"Maak een nieuw ticket aan in het systeem."</t>
+  </si>
+  <si>
+    <t>"All tickets"</t>
+  </si>
+  <si>
+    <t>"Alle tickets"</t>
+  </si>
+  <si>
+    <t>"Shows a list with all existing tickets."</t>
+  </si>
+  <si>
+    <t>"Toont een lijst van alle bestaande tickets."</t>
+  </si>
+  <si>
+    <t>"Create"</t>
+  </si>
+  <si>
+    <t>"Maak aan"</t>
+  </si>
+  <si>
+    <t>"Toon ticket"</t>
+  </si>
+  <si>
+    <t>"Show ticket"</t>
+  </si>
+  <si>
+    <t>"Show the details of a ticket."</t>
+  </si>
+  <si>
+    <t>"Geeft de details van één ticket."</t>
+  </si>
+  <si>
+    <t>"TicketNumber"</t>
+  </si>
+  <si>
+    <t>"Ticketnummer"</t>
+  </si>
+  <si>
+    <t>MVC_h_AboutTitle</t>
+  </si>
+  <si>
+    <t>MVC_h_AboutContent</t>
+  </si>
+  <si>
+    <t>MVC_h_ContactTitle</t>
+  </si>
+  <si>
+    <t>MVC_h_ContactPhoneTitle</t>
+  </si>
+  <si>
+    <t>MVC_h_ContactPhoneContent</t>
+  </si>
+  <si>
+    <t>MVC_h_Support</t>
+  </si>
+  <si>
+    <t>MVC_h_Marketing</t>
+  </si>
+  <si>
+    <t>MVC_h_IndexTitle</t>
+  </si>
+  <si>
+    <t>MVC_h_SupportCenter</t>
+  </si>
+  <si>
+    <t>MVC_h_WelcomeMssgIndex</t>
+  </si>
+  <si>
+    <t>MVC_h_NewTicket</t>
+  </si>
+  <si>
+    <t>MVC_h_NewTicketInfo</t>
+  </si>
+  <si>
+    <t>MVC_h_ActionLinkCreate</t>
+  </si>
+  <si>
+    <t>MVC_h_AllTickets</t>
+  </si>
+  <si>
+    <t>MVC_h_AllTicketsInfo</t>
+  </si>
+  <si>
+    <t>MVC_h_ActionLinkAllTickets</t>
+  </si>
+  <si>
+    <t>MVC_h_ShowTicket</t>
+  </si>
+  <si>
+    <t>MVC_h_ShowTicketInfo</t>
+  </si>
+  <si>
+    <t>MVC_h_FormIdLabel</t>
+  </si>
+  <si>
+    <t>MVC_h_FormBttnValue</t>
+  </si>
+  <si>
+    <t>MVC_s_ErrorTitle</t>
+  </si>
+  <si>
+    <t>"Error"</t>
+  </si>
+  <si>
+    <t>"Fout"</t>
+  </si>
+  <si>
+    <t>MVC_s_ErrorH1</t>
+  </si>
+  <si>
+    <t>"Error."</t>
+  </si>
+  <si>
+    <t>"Fout."</t>
+  </si>
+  <si>
+    <t>MVC_s_ErrorH2</t>
+  </si>
+  <si>
+    <t>"An error ocurres while processing your request."</t>
+  </si>
+  <si>
+    <t>"Er is een fout opgetreden tijdens het verwerken van je aanvraag."</t>
+  </si>
+  <si>
+    <t>MVC_t_ActionLickBack</t>
+  </si>
+  <si>
+    <t>"Back to List"</t>
+  </si>
+  <si>
+    <t>"Terug naar de lijst"</t>
+  </si>
+  <si>
+    <t>MVC_t_DeleteBttn</t>
+  </si>
+  <si>
+    <t>"Delete"</t>
+  </si>
+  <si>
+    <t>"Verwijder"</t>
+  </si>
+  <si>
+    <t>MVC_t_DetailsTitle</t>
+  </si>
+  <si>
+    <t>"Details"</t>
+  </si>
+  <si>
+    <t>MVC_t_DeleteH2</t>
+  </si>
+  <si>
+    <t>"Are you sure you want to delete this?"</t>
+  </si>
+  <si>
+    <t>"Weet je zeker dat je dit wilt verwijderen?"</t>
+  </si>
+  <si>
+    <t>"Ticket"</t>
+  </si>
+  <si>
+    <t>MVC_t_TicketH4</t>
+  </si>
+  <si>
+    <t>MVC_t_ActionLinkEdit</t>
+  </si>
+  <si>
+    <t>"Edit"</t>
+  </si>
+  <si>
+    <t>"Pas aan"</t>
+  </si>
+  <si>
+    <t>MVC_t_LoadAnswerBttn</t>
+  </si>
+  <si>
+    <t>"Load answers"</t>
+  </si>
+  <si>
+    <t>"Laad antwoorden"</t>
+  </si>
+  <si>
+    <t>MVC_t_IsClientResponse</t>
+  </si>
+  <si>
+    <t>"IsClientResponse"</t>
+  </si>
+  <si>
+    <t>"Is door een klant beantwoord"</t>
+  </si>
+  <si>
+    <t>MVC_t_Send</t>
+  </si>
+  <si>
+    <t>"Send"</t>
+  </si>
+  <si>
+    <t>"Verzenden"</t>
+  </si>
+  <si>
+    <t>MVC_t_Alert</t>
+  </si>
+  <si>
+    <t>"Oeps, something went wrong!"</t>
+  </si>
+  <si>
+    <t>"Oeps, er liep iets verkeerd!"</t>
+  </si>
+  <si>
+    <t>MVC_t_SaveBttn</t>
+  </si>
+  <si>
+    <t>"Save"</t>
+  </si>
+  <si>
+    <t>"Sla op"</t>
+  </si>
+  <si>
+    <t>MVC_t_IndexTitle</t>
+  </si>
+  <si>
+    <t>"Index"</t>
+  </si>
+  <si>
+    <t>MVC_t_CreateNew</t>
+  </si>
+  <si>
+    <t>"Create New"</t>
+  </si>
+  <si>
+    <t>"Aanmaken"</t>
   </si>
 </sst>
 </file>
@@ -398,18 +752,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C5"/>
+  <dimension ref="A1:C43"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
+      <pane ySplit="1" topLeftCell="A23" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A44" sqref="A44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="12.6640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.77734375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="26.77734375" customWidth="1"/>
+    <col min="2" max="2" width="57.6640625" customWidth="1"/>
+    <col min="3" max="3" width="54.77734375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.3">
@@ -423,8 +777,467 @@
         <v>0</v>
       </c>
     </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C3" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>8</v>
+      </c>
+      <c r="B4" t="s">
+        <v>9</v>
+      </c>
+      <c r="C4" t="s">
+        <v>10</v>
+      </c>
+    </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="B5" s="1"/>
+      <c r="A5" t="s">
+        <v>12</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C5" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>15</v>
+      </c>
+      <c r="B6" t="s">
+        <v>16</v>
+      </c>
+      <c r="C6" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>17</v>
+      </c>
+      <c r="B7" t="s">
+        <v>18</v>
+      </c>
+      <c r="C7" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>56</v>
+      </c>
+      <c r="B8" t="s">
+        <v>21</v>
+      </c>
+      <c r="C8" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>57</v>
+      </c>
+      <c r="B9" t="s">
+        <v>24</v>
+      </c>
+      <c r="C9" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>58</v>
+      </c>
+      <c r="B10" t="s">
+        <v>23</v>
+      </c>
+      <c r="C10" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>59</v>
+      </c>
+      <c r="B11" t="s">
+        <v>26</v>
+      </c>
+      <c r="C11" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>60</v>
+      </c>
+      <c r="B12" t="s">
+        <v>28</v>
+      </c>
+      <c r="C12" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
+        <v>61</v>
+      </c>
+      <c r="B13" t="s">
+        <v>30</v>
+      </c>
+      <c r="C13" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
+        <v>62</v>
+      </c>
+      <c r="B14" t="s">
+        <v>32</v>
+      </c>
+      <c r="C14" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
+        <v>63</v>
+      </c>
+      <c r="B15" t="s">
+        <v>34</v>
+      </c>
+      <c r="C15" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A16" t="s">
+        <v>64</v>
+      </c>
+      <c r="B16" t="s">
+        <v>36</v>
+      </c>
+      <c r="C16" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A17" t="s">
+        <v>65</v>
+      </c>
+      <c r="B17" t="s">
+        <v>38</v>
+      </c>
+      <c r="C17" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A18" t="s">
+        <v>66</v>
+      </c>
+      <c r="B18" t="s">
+        <v>40</v>
+      </c>
+      <c r="C18" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A19" t="s">
+        <v>67</v>
+      </c>
+      <c r="B19" t="s">
+        <v>42</v>
+      </c>
+      <c r="C19" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A20" t="s">
+        <v>68</v>
+      </c>
+      <c r="B20" t="s">
+        <v>48</v>
+      </c>
+      <c r="C20" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A21" t="s">
+        <v>69</v>
+      </c>
+      <c r="B21" t="s">
+        <v>44</v>
+      </c>
+      <c r="C21" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A22" t="s">
+        <v>70</v>
+      </c>
+      <c r="B22" t="s">
+        <v>46</v>
+      </c>
+      <c r="C22" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A23" t="s">
+        <v>71</v>
+      </c>
+      <c r="B23" t="s">
+        <v>44</v>
+      </c>
+      <c r="C23" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A24" t="s">
+        <v>72</v>
+      </c>
+      <c r="B24" t="s">
+        <v>50</v>
+      </c>
+      <c r="C24" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A25" t="s">
+        <v>73</v>
+      </c>
+      <c r="B25" t="s">
+        <v>52</v>
+      </c>
+      <c r="C25" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A26" t="s">
+        <v>74</v>
+      </c>
+      <c r="B26" t="s">
+        <v>54</v>
+      </c>
+      <c r="C26" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A27" t="s">
+        <v>75</v>
+      </c>
+      <c r="B27" t="s">
+        <v>51</v>
+      </c>
+      <c r="C27" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A28" t="s">
+        <v>76</v>
+      </c>
+      <c r="B28" t="s">
+        <v>77</v>
+      </c>
+      <c r="C28" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A29" t="s">
+        <v>79</v>
+      </c>
+      <c r="B29" t="s">
+        <v>80</v>
+      </c>
+      <c r="C29" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A30" t="s">
+        <v>82</v>
+      </c>
+      <c r="B30" t="s">
+        <v>83</v>
+      </c>
+      <c r="C30" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A31" t="s">
+        <v>85</v>
+      </c>
+      <c r="B31" t="s">
+        <v>86</v>
+      </c>
+      <c r="C31" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A32" t="s">
+        <v>88</v>
+      </c>
+      <c r="B32" t="s">
+        <v>89</v>
+      </c>
+      <c r="C32" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A33" t="s">
+        <v>93</v>
+      </c>
+      <c r="B33" t="s">
+        <v>94</v>
+      </c>
+      <c r="C33" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A34" t="s">
+        <v>97</v>
+      </c>
+      <c r="B34" t="s">
+        <v>96</v>
+      </c>
+      <c r="C34" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A35" t="s">
+        <v>91</v>
+      </c>
+      <c r="B35" t="s">
+        <v>92</v>
+      </c>
+      <c r="C35" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A36" t="s">
+        <v>98</v>
+      </c>
+      <c r="B36" t="s">
+        <v>99</v>
+      </c>
+      <c r="C36" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A37" t="s">
+        <v>101</v>
+      </c>
+      <c r="B37" t="s">
+        <v>102</v>
+      </c>
+      <c r="C37" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A38" t="s">
+        <v>104</v>
+      </c>
+      <c r="B38" t="s">
+        <v>105</v>
+      </c>
+      <c r="C38" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A39" t="s">
+        <v>107</v>
+      </c>
+      <c r="B39" t="s">
+        <v>108</v>
+      </c>
+      <c r="C39" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A40" t="s">
+        <v>110</v>
+      </c>
+      <c r="B40" t="s">
+        <v>111</v>
+      </c>
+      <c r="C40" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A41" t="s">
+        <v>113</v>
+      </c>
+      <c r="B41" t="s">
+        <v>114</v>
+      </c>
+      <c r="C41" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A42" t="s">
+        <v>116</v>
+      </c>
+      <c r="B42" t="s">
+        <v>117</v>
+      </c>
+      <c r="C42" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A43" t="s">
+        <v>118</v>
+      </c>
+      <c r="B43" t="s">
+        <v>119</v>
+      </c>
+      <c r="C43" t="s">
+        <v>120</v>
+      </c>
     </row>
   </sheetData>
   <autoFilter ref="A1:C6"/>

</xml_diff>